<commit_message>
edit userController for test
</commit_message>
<xml_diff>
--- a/src/main/resources/data/products.xlsx
+++ b/src/main/resources/data/products.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
   <si>
-    <t>stri</t>
+    <t>laptop acer</t>
   </si>
 </sst>
 </file>
@@ -76,10 +76,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="n" s="0">
-        <v>10.0</v>
+        <v>100.0</v>
       </c>
       <c r="D1" t="n" s="0">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>